<commit_message>
Update Excel files from OneDrive - Wed May  7 18:46:18 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Certifications.xlsx
+++ b/data/Certifications.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28830"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="87" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FB9279BB-9D07-41FA-8512-B3797641530F}"/>
+  <xr:revisionPtr revIDLastSave="92" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BDBE2C7D-75EB-4500-B3CA-808691F66DC0}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ref" sheetId="1" r:id="rId1"/>
@@ -111,7 +111,7 @@
     <t>NOTES</t>
   </si>
   <si>
-    <t>f</t>
+    <t>OK</t>
   </si>
   <si>
     <t>START_DATE</t>
@@ -633,7 +633,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -664,13 +664,13 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="D2" s="1">
         <v>37257</v>

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Thu May  8 09:57:08 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Certifications.xlsx
+++ b/data/Certifications.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28906"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="92" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BDBE2C7D-75EB-4500-B3CA-808691F66DC0}"/>
+  <xr:revisionPtr revIDLastSave="103" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D2494284-97C6-446D-9ED9-F502D2C33A4A}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="28">
   <si>
     <t>PRODUCT</t>
   </si>
@@ -111,7 +111,10 @@
     <t>NOTES</t>
   </si>
   <si>
-    <t>OK</t>
+    <t>M10_HYPERSOL_108</t>
+  </si>
+  <si>
+    <t>16/12/2024</t>
   </si>
   <si>
     <t>START_DATE</t>
@@ -127,13 +130,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="-Apple-System"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -158,7 +167,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -633,7 +642,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -663,48 +672,42 @@
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
+      <c r="A2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="1">
-        <v>37257</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="D2" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="1">
-        <v>37257</v>
-      </c>
-      <c r="E3" t="s">
-        <v>23</v>
+        <v>7</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A1048576" xr:uid="{1258B334-D16A-4B05-BB00-CC64FB57C33B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A4:A1048576" xr:uid="{1258B334-D16A-4B05-BB00-CC64FB57C33B}">
       <formula1>product_list</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B1048576" xr:uid="{1E2C7863-4447-4C30-B8EC-087CA23FA7DC}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B1048576" xr:uid="{1E2C7863-4447-4C30-B8EC-087CA23FA7DC}">
       <formula1>certification_list</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C1048576" xr:uid="{2BADC456-64E9-47CF-9D68-A5D0EE4884B2}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:C1048576" xr:uid="{2BADC456-64E9-47CF-9D68-A5D0EE4884B2}">
       <formula1>agency_list</formula1>
     </dataValidation>
   </dataValidations>
@@ -744,10 +747,10 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
@@ -800,7 +803,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E1" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Thu May  8 10:23:27 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Certifications.xlsx
+++ b/data/Certifications.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28906"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="103" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D2494284-97C6-446D-9ED9-F502D2C33A4A}"/>
+  <xr:revisionPtr revIDLastSave="197" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B8ABEB73-A519-4758-8A79-D8AB8A268DAB}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="45">
   <si>
     <t>PRODUCT</t>
   </si>
@@ -115,6 +115,59 @@
   </si>
   <si>
     <t>16/12/2024</t>
+  </si>
+  <si>
+    <t>M10_HYPERSOL_120</t>
+  </si>
+  <si>
+    <t>G12R_HYPERSOL_132</t>
+  </si>
+  <si>
+    <t>IEC 62716</t>
+  </si>
+  <si>
+    <t>27/11/2024</t>
+  </si>
+  <si>
+    <t>M10_HYPERSOL_144</t>
+  </si>
+  <si>
+    <t>M10_HYPERSOL_132</t>
+  </si>
+  <si>
+    <t>TRANSPORTATION TEST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+09/01/2025</t>
+  </si>
+  <si>
+    <t>565-610</t>
+  </si>
+  <si>
+    <t>IEC 62804</t>
+  </si>
+  <si>
+    <t>IEC 61701</t>
+  </si>
+  <si>
+    <t>KIWA PVEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+24/03/2025</t>
+  </si>
+  <si>
+    <t>570-595</t>
+  </si>
+  <si>
+    <t>G12_HYPERSOL_132</t>
+  </si>
+  <si>
+    <t>pvel</t>
+  </si>
+  <si>
+    <t>600-625</t>
   </si>
   <si>
     <t>START_DATE</t>
@@ -145,15 +198,21 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFAFAFA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -161,13 +220,38 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="6"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="6"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFF0F0F0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -186,8 +270,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2A9E0FF9-41E1-41C8-9CB9-5AC8D94915A5}" name="Table1" displayName="Table1" ref="A1:E3" insertRowShift="1" totalsRowShown="0">
-  <autoFilter ref="A1:E3" xr:uid="{2A9E0FF9-41E1-41C8-9CB9-5AC8D94915A5}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2A9E0FF9-41E1-41C8-9CB9-5AC8D94915A5}" name="Table1" displayName="Table1" ref="A1:E23" insertRowShift="1" totalsRowShown="0">
+  <autoFilter ref="A1:E23" xr:uid="{2A9E0FF9-41E1-41C8-9CB9-5AC8D94915A5}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{CCE7B811-5136-4C3F-BCF9-4903D9F6FE03}" name="PRODUCT"/>
     <tableColumn id="2" xr3:uid="{AE958FA9-F96A-463E-A663-292B1D1342EE}" name="CERTIFICATION"/>
@@ -639,15 +723,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E7B6282-5A9A-496F-9B95-80914196A9BC}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A1048558" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
     <col min="2" max="2" width="17.28515625" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" customWidth="1"/>
     <col min="4" max="4" width="21.140625" customWidth="1"/>
@@ -699,15 +783,304 @@
         <v>24</v>
       </c>
     </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="33.75">
+      <c r="A15" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="3">
+        <v>45424</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="3">
+        <v>45638</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" s="3">
+        <v>45901</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="33.75">
+      <c r="A22" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E22" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" s="3">
+        <v>45780</v>
+      </c>
+      <c r="E23" t="s">
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A4:A1048576" xr:uid="{1258B334-D16A-4B05-BB00-CC64FB57C33B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A24:A1048576" xr:uid="{1258B334-D16A-4B05-BB00-CC64FB57C33B}">
       <formula1>product_list</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B1048576" xr:uid="{1E2C7863-4447-4C30-B8EC-087CA23FA7DC}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B14 B22:B1048576" xr:uid="{1E2C7863-4447-4C30-B8EC-087CA23FA7DC}">
       <formula1>certification_list</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:C1048576" xr:uid="{2BADC456-64E9-47CF-9D68-A5D0EE4884B2}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:C16 C18:C1048576" xr:uid="{2BADC456-64E9-47CF-9D68-A5D0EE4884B2}">
       <formula1>agency_list</formula1>
     </dataValidation>
   </dataValidations>
@@ -747,10 +1120,10 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="E1" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
@@ -803,7 +1176,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="E1" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Thu May  8 10:27:07 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Certifications.xlsx
+++ b/data/Certifications.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28906"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="197" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B8ABEB73-A519-4758-8A79-D8AB8A268DAB}"/>
+  <xr:revisionPtr revIDLastSave="198" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0A81D556-31BC-4230-AA53-A822165FB14D}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -725,8 +725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E7B6282-5A9A-496F-9B95-80914196A9BC}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1048558" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1073,7 +1073,7 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="3">
+  <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A24:A1048576" xr:uid="{1258B334-D16A-4B05-BB00-CC64FB57C33B}">
       <formula1>product_list</formula1>
     </dataValidation>
@@ -1082,6 +1082,10 @@
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:C16 C18:C1048576" xr:uid="{2BADC456-64E9-47CF-9D68-A5D0EE4884B2}">
       <formula1>agency_list</formula1>
+    </dataValidation>
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{AAE86110-D93C-4137-B15E-64716D240337}">
+      <formula1>36892</formula1>
+      <formula2>73050</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Thu May  8 11:34:38 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Certifications.xlsx
+++ b/data/Certifications.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28906"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28830"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="198" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0A81D556-31BC-4230-AA53-A822165FB14D}"/>
+  <xr:revisionPtr revIDLastSave="200" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9C848285-91C6-4590-B234-F9C8144F6251}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="44">
   <si>
     <t>PRODUCT</t>
   </si>
@@ -152,10 +152,6 @@
   </si>
   <si>
     <t>KIWA PVEL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-24/03/2025</t>
   </si>
   <si>
     <t>570-595</t>
@@ -244,12 +240,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -725,8 +724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E7B6282-5A9A-496F-9B95-80914196A9BC}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1038,7 +1037,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="33.75">
+    <row r="22" spans="1:5" ht="14.25">
       <c r="A22" s="2" t="s">
         <v>29</v>
       </c>
@@ -1048,19 +1047,19 @@
       <c r="C22" t="s">
         <v>36</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D22" s="5">
+        <v>45740</v>
+      </c>
+      <c r="E22" t="s">
         <v>37</v>
-      </c>
-      <c r="E22" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" t="s">
         <v>39</v>
-      </c>
-      <c r="B23" t="s">
-        <v>40</v>
       </c>
       <c r="C23" t="s">
         <v>36</v>
@@ -1069,7 +1068,7 @@
         <v>45780</v>
       </c>
       <c r="E23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1124,10 +1123,10 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" t="s">
         <v>42</v>
-      </c>
-      <c r="E1" t="s">
-        <v>43</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
@@ -1180,7 +1179,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E1" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Mon May 12 05:14:55 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Certifications.xlsx
+++ b/data/Certifications.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28906"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="200" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9C848285-91C6-4590-B234-F9C8144F6251}"/>
+  <xr:revisionPtr revIDLastSave="295" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B88556A9-664D-4F84-B1C6-16ECE2C83CEF}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="56">
   <si>
     <t>PRODUCT</t>
   </si>
@@ -164,6 +164,42 @@
   </si>
   <si>
     <t>600-625</t>
+  </si>
+  <si>
+    <t>G12_PARADEA_120</t>
+  </si>
+  <si>
+    <t>BIS 14286</t>
+  </si>
+  <si>
+    <t>M10_PARADEA_132</t>
+  </si>
+  <si>
+    <t>M10_PARADEA_144</t>
+  </si>
+  <si>
+    <t>G12_PARADEA_132</t>
+  </si>
+  <si>
+    <t>M10_PARADEA_108</t>
+  </si>
+  <si>
+    <t>M10_PARADEA_156</t>
+  </si>
+  <si>
+    <t>M10_PARADEA_120</t>
+  </si>
+  <si>
+    <t>M10_PREXOS_108</t>
+  </si>
+  <si>
+    <t>CHENNAI</t>
+  </si>
+  <si>
+    <t>M10_PREXOS_120</t>
+  </si>
+  <si>
+    <t>M10_PREXOS_144</t>
   </si>
   <si>
     <t>START_DATE</t>
@@ -240,7 +276,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -251,6 +287,7 @@
     <xf numFmtId="14" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -269,8 +306,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2A9E0FF9-41E1-41C8-9CB9-5AC8D94915A5}" name="Table1" displayName="Table1" ref="A1:E23" insertRowShift="1" totalsRowShown="0">
-  <autoFilter ref="A1:E23" xr:uid="{2A9E0FF9-41E1-41C8-9CB9-5AC8D94915A5}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2A9E0FF9-41E1-41C8-9CB9-5AC8D94915A5}" name="Table1" displayName="Table1" ref="A1:E44" insertRowShift="1" totalsRowShown="0">
+  <autoFilter ref="A1:E44" xr:uid="{2A9E0FF9-41E1-41C8-9CB9-5AC8D94915A5}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{CCE7B811-5136-4C3F-BCF9-4903D9F6FE03}" name="PRODUCT"/>
     <tableColumn id="2" xr3:uid="{AE958FA9-F96A-463E-A663-292B1D1342EE}" name="CERTIFICATION"/>
@@ -722,10 +759,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E7B6282-5A9A-496F-9B95-80914196A9BC}">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1071,12 +1108,318 @@
         <v>40</v>
       </c>
     </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="6">
+        <v>45320</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="6">
+        <v>45702</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" s="6">
+        <v>45167</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" s="6">
+        <v>45190</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B28" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" s="6">
+        <v>45190</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" s="6">
+        <v>45190</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B30" t="s">
+        <v>14</v>
+      </c>
+      <c r="C30" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30" s="6">
+        <v>45623</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B31" t="s">
+        <v>18</v>
+      </c>
+      <c r="C31" t="s">
+        <v>11</v>
+      </c>
+      <c r="D31" s="6">
+        <v>45623</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B32" t="s">
+        <v>27</v>
+      </c>
+      <c r="C32" t="s">
+        <v>11</v>
+      </c>
+      <c r="D32" s="6">
+        <v>45623</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B33" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33" s="6">
+        <v>45645</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B34" t="s">
+        <v>10</v>
+      </c>
+      <c r="C34" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34" s="6">
+        <v>45642</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B35" t="s">
+        <v>6</v>
+      </c>
+      <c r="C35" t="s">
+        <v>7</v>
+      </c>
+      <c r="D35" s="6">
+        <v>45642</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B36" t="s">
+        <v>10</v>
+      </c>
+      <c r="C36" t="s">
+        <v>7</v>
+      </c>
+      <c r="D36" s="6">
+        <v>45642</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B37" t="s">
+        <v>6</v>
+      </c>
+      <c r="C37" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" s="6">
+        <v>45644</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B38" t="s">
+        <v>10</v>
+      </c>
+      <c r="C38" t="s">
+        <v>7</v>
+      </c>
+      <c r="D38" s="6">
+        <v>45644</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B39" t="s">
+        <v>6</v>
+      </c>
+      <c r="C39" t="s">
+        <v>7</v>
+      </c>
+      <c r="D39" s="6">
+        <v>45642</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B40" t="s">
+        <v>10</v>
+      </c>
+      <c r="C40" t="s">
+        <v>7</v>
+      </c>
+      <c r="D40" s="6">
+        <v>45642</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B41" t="s">
+        <v>10</v>
+      </c>
+      <c r="C41" t="s">
+        <v>7</v>
+      </c>
+      <c r="D41" s="6">
+        <v>45426</v>
+      </c>
+      <c r="E41" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B42" t="s">
+        <v>42</v>
+      </c>
+      <c r="C42" t="s">
+        <v>7</v>
+      </c>
+      <c r="D42" s="6">
+        <v>45457</v>
+      </c>
+      <c r="E42" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B43" t="s">
+        <v>42</v>
+      </c>
+      <c r="C43" t="s">
+        <v>7</v>
+      </c>
+      <c r="D43" s="6">
+        <v>45457</v>
+      </c>
+      <c r="E43" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B44" t="s">
+        <v>42</v>
+      </c>
+      <c r="C44" t="s">
+        <v>7</v>
+      </c>
+      <c r="D44" s="6">
+        <v>45457</v>
+      </c>
+      <c r="E44" t="s">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A24:A1048576" xr:uid="{1258B334-D16A-4B05-BB00-CC64FB57C33B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A45:A1048576" xr:uid="{1258B334-D16A-4B05-BB00-CC64FB57C33B}">
       <formula1>product_list</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B14 B22:B1048576" xr:uid="{1E2C7863-4447-4C30-B8EC-087CA23FA7DC}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B14 B22:B23 B25:B1048576" xr:uid="{1E2C7863-4447-4C30-B8EC-087CA23FA7DC}">
       <formula1>certification_list</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:C16 C18:C1048576" xr:uid="{2BADC456-64E9-47CF-9D68-A5D0EE4884B2}">
@@ -1123,10 +1466,10 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="E1" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
@@ -1179,7 +1522,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="E1" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Update Excel files from OneDrive - Tue May 20 06:40:35 UTC 2025
</commit_message>
<xml_diff>
--- a/data/Certifications.xlsx
+++ b/data/Certifications.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28906"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28914"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="295" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B88556A9-664D-4F84-B1C6-16ECE2C83CEF}"/>
+  <xr:revisionPtr revIDLastSave="311" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2BC5AADF-2C94-4775-AA50-B3AC80D9BA5E}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ref" sheetId="1" r:id="rId1"/>
@@ -16,6 +16,7 @@
   <definedNames>
     <definedName name="agency_list">ref!$C$2:$C$1048576</definedName>
     <definedName name="certification_list">ref!$B$2:$B$1048576</definedName>
+    <definedName name="plant_name">ref!$F$2:$F$1048576</definedName>
     <definedName name="priority_list">ref!$E$2:$E$1048576</definedName>
     <definedName name="product_list">ref!$A$2:$A$1048576</definedName>
   </definedNames>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="59">
   <si>
     <t>PRODUCT</t>
   </si>
@@ -57,6 +58,9 @@
     <t>PRIORITY</t>
   </si>
   <si>
+    <t>PLANT_NAME</t>
+  </si>
+  <si>
     <t>HYPERSOL</t>
   </si>
   <si>
@@ -69,6 +73,9 @@
     <t>HIGH</t>
   </si>
   <si>
+    <t>FALTA</t>
+  </si>
+  <si>
     <t>SURYAVA</t>
   </si>
   <si>
@@ -81,6 +88,9 @@
     <t>MEDIUM</t>
   </si>
   <si>
+    <t>CHENNAI</t>
+  </si>
+  <si>
     <t>PARADEA</t>
   </si>
   <si>
@@ -109,6 +119,9 @@
   </si>
   <si>
     <t>NOTES</t>
+  </si>
+  <si>
+    <t>WATTPEAK</t>
   </si>
   <si>
     <t>M10_HYPERSOL_108</t>
@@ -191,9 +204,6 @@
   </si>
   <si>
     <t>M10_PREXOS_108</t>
-  </si>
-  <si>
-    <t>CHENNAI</t>
   </si>
   <si>
     <t>M10_PREXOS_120</t>
@@ -306,43 +316,49 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2A9E0FF9-41E1-41C8-9CB9-5AC8D94915A5}" name="Table1" displayName="Table1" ref="A1:E44" insertRowShift="1" totalsRowShown="0">
-  <autoFilter ref="A1:E44" xr:uid="{2A9E0FF9-41E1-41C8-9CB9-5AC8D94915A5}"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2A9E0FF9-41E1-41C8-9CB9-5AC8D94915A5}" name="Table1" displayName="Table1" ref="A1:G44" insertRowShift="1" totalsRowShown="0">
+  <autoFilter ref="A1:G44" xr:uid="{2A9E0FF9-41E1-41C8-9CB9-5AC8D94915A5}"/>
+  <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{CCE7B811-5136-4C3F-BCF9-4903D9F6FE03}" name="PRODUCT"/>
     <tableColumn id="2" xr3:uid="{AE958FA9-F96A-463E-A663-292B1D1342EE}" name="CERTIFICATION"/>
     <tableColumn id="3" xr3:uid="{F4B99087-8481-46B7-BDF7-73026FD87424}" name="AGENCY"/>
     <tableColumn id="4" xr3:uid="{DD7D7010-2DDE-4BC9-8FD4-54830477DF09}" name="COMPLETION_DATE"/>
     <tableColumn id="5" xr3:uid="{AA156137-B7F1-469E-B170-D94F4C71FD49}" name="NOTES"/>
+    <tableColumn id="6" xr3:uid="{BE80CEBE-18D1-4ABF-A2FE-D92D67983786}" name="WATTPEAK"/>
+    <tableColumn id="7" xr3:uid="{12D8457E-A22A-48BC-8587-969FE30CBB83}" name="PLANT_NAME"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9AAFCA8D-AC81-4C87-9708-8A106E7B6770}" name="Table2" displayName="Table2" ref="A1:F2" insertRow="1" insertRowShift="1" totalsRowShown="0">
-  <autoFilter ref="A1:F2" xr:uid="{9AAFCA8D-AC81-4C87-9708-8A106E7B6770}"/>
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9AAFCA8D-AC81-4C87-9708-8A106E7B6770}" name="Table2" displayName="Table2" ref="A1:H2" insertRow="1" insertRowShift="1" totalsRowShown="0">
+  <autoFilter ref="A1:H2" xr:uid="{9AAFCA8D-AC81-4C87-9708-8A106E7B6770}"/>
+  <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{C65E5835-CFC5-487C-9275-F9F49E43E73B}" name="PRODUCT"/>
     <tableColumn id="2" xr3:uid="{B7DF1DCC-1984-4943-8FC4-99726A7BFFDE}" name="CERTIFICATION"/>
     <tableColumn id="3" xr3:uid="{5790D4C3-C6B6-42FF-A866-95FF544740AA}" name="AGENCY"/>
     <tableColumn id="4" xr3:uid="{EAE5D17D-CE04-4D38-A536-6163CE793C12}" name="START_DATE"/>
     <tableColumn id="5" xr3:uid="{DE19768B-786E-4A8F-BC36-A9F658FEBA2F}" name="EXPECTED_COMPLETION"/>
     <tableColumn id="6" xr3:uid="{0A039712-CCD0-49BC-9F28-A1FAB07A7F29}" name="STATUS"/>
+    <tableColumn id="7" xr3:uid="{22B5B808-17EF-4C52-BC81-BE20915F7BA8}" name="WATTPEAK"/>
+    <tableColumn id="8" xr3:uid="{A42085E3-1B7B-439D-A3F6-32764B8F0ADD}" name="PLANT_NAME"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7824F395-1AD8-42B6-8FC3-0E149DA5EA8E}" name="Table3" displayName="Table3" ref="A1:E2" insertRow="1" insertRowShift="1" totalsRowShown="0">
-  <autoFilter ref="A1:E2" xr:uid="{7824F395-1AD8-42B6-8FC3-0E149DA5EA8E}"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7824F395-1AD8-42B6-8FC3-0E149DA5EA8E}" name="Table3" displayName="Table3" ref="A1:G2" insertRow="1" insertRowShift="1" totalsRowShown="0">
+  <autoFilter ref="A1:G2" xr:uid="{7824F395-1AD8-42B6-8FC3-0E149DA5EA8E}"/>
+  <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{2209C0B5-08F7-48F4-8375-2FE1714E2A0F}" name="PRODUCT"/>
     <tableColumn id="2" xr3:uid="{76213258-157E-433D-9FDC-F4B4877185A9}" name="CERTIFICATION"/>
     <tableColumn id="3" xr3:uid="{27C8EBA6-8578-41B7-A44A-2CA521DFE411}" name="AGENCY"/>
     <tableColumn id="4" xr3:uid="{D89C980D-83B6-4E41-96D0-0F4625ECF677}" name="PLANNED_START"/>
     <tableColumn id="5" xr3:uid="{54ED6631-37EA-4753-8A15-D2552DB3ED2F}" name="PRIORITY"/>
+    <tableColumn id="6" xr3:uid="{8A251ACF-C753-408B-B051-439E7EC89718}" name="WATTPEAK"/>
+    <tableColumn id="7" xr3:uid="{CBD1742E-48EF-427F-9ED0-D906D4291E65}" name="PLANT_NAME"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -665,10 +681,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A1048557" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -677,7 +693,7 @@
     <col min="3" max="3" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -693,63 +709,72 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -759,10 +784,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E7B6282-5A9A-496F-9B95-80914196A9BC}">
-  <dimension ref="A1:E44"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -774,7 +799,7 @@
     <col min="5" max="5" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -785,637 +810,646 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" t="s">
         <v>21</v>
       </c>
-      <c r="E1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" t="s">
-        <v>18</v>
-      </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C12" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C14" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="33.75">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="33.75">
       <c r="A15" s="2" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C15" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="B16" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C16" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D16" s="3">
         <v>45424</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:6">
       <c r="A17" s="2" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D17" s="3">
         <v>45638</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:6">
       <c r="A18" s="2" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C18" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" s="2" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" s="2" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C20" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D20" s="3">
         <v>45901</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:6">
       <c r="A21" s="2" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C21" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="14.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="14.25">
       <c r="A22" s="2" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B22" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C22" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D22" s="5">
         <v>45740</v>
       </c>
-      <c r="E22" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
+      <c r="F22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B23" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C23" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D23" s="3">
         <v>45780</v>
       </c>
-      <c r="E23" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
+      <c r="F23" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C24" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D24" s="6">
         <v>45320</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:6">
       <c r="A25" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B25" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C25" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D25" s="6">
         <v>45702</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:6">
       <c r="A26" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B26" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C26" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D26" s="6">
         <v>45167</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:6">
       <c r="A27" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B27" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C27" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D27" s="6">
         <v>45190</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:6">
       <c r="A28" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B28" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C28" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D28" s="6">
         <v>45190</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:6">
       <c r="A29" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B29" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C29" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D29" s="6">
         <v>45190</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:6">
       <c r="A30" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B30" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C30" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D30" s="6">
         <v>45623</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:6">
       <c r="A31" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B31" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C31" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D31" s="6">
         <v>45623</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:6">
       <c r="A32" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B32" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C32" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D32" s="6">
         <v>45623</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:7">
       <c r="A33" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B33" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C33" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D33" s="6">
         <v>45645</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:7">
       <c r="A34" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B34" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C34" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D34" s="6">
         <v>45642</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:7">
       <c r="A35" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B35" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C35" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D35" s="6">
         <v>45642</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:7">
       <c r="A36" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B36" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C36" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D36" s="6">
         <v>45642</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:7">
       <c r="A37" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B37" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C37" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D37" s="6">
         <v>45644</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:7">
       <c r="A38" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B38" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C38" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D38" s="6">
         <v>45644</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:7">
       <c r="A39" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B39" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C39" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D39" s="6">
         <v>45642</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:7">
       <c r="A40" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B40" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C40" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D40" s="6">
         <v>45642</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:7">
       <c r="A41" s="1" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B41" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C41" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D41" s="6">
         <v>45426</v>
       </c>
-      <c r="E41" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5">
+      <c r="G41" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
       <c r="A42" s="1" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B42" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C42" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D42" s="6">
         <v>45457</v>
       </c>
-      <c r="E42" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5">
+      <c r="G42" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
       <c r="A43" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B43" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C43" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D43" s="6">
         <v>45457</v>
       </c>
-      <c r="E43" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5">
+      <c r="G43" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
       <c r="A44" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B44" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C44" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D44" s="6">
         <v>45457</v>
       </c>
-      <c r="E44" t="s">
-        <v>50</v>
+      <c r="G44" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="4">
+  <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A45:A1048576" xr:uid="{1258B334-D16A-4B05-BB00-CC64FB57C33B}">
       <formula1>product_list</formula1>
     </dataValidation>
@@ -1429,6 +1463,9 @@
       <formula1>36892</formula1>
       <formula2>73050</formula2>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576" xr:uid="{969DE66B-3AE6-4A53-840D-9B3EA3BAAB3E}">
+      <formula1>plant_name</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -1439,10 +1476,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D7BD586-25CC-4351-8A28-721817832F65}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1455,7 +1492,7 @@
     <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1466,13 +1503,19 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="E1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -1496,10 +1539,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BB94438-1C9D-4DF3-A226-9E18738BB2DC}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E1"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1511,7 +1554,7 @@
     <col min="5" max="5" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1522,10 +1565,16 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E1" t="s">
         <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>